<commit_message>
working for talkmap (manual entry)
</commit_message>
<xml_diff>
--- a/markdown_generator/talks.xlsx
+++ b/markdown_generator/talks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuk/git-web/stsykw.github.io/markdown_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4130B890-422B-1649-8E4F-BF222FF11743}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1025E0-CBE6-364F-A45A-1A9EF4A0D193}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="460" windowWidth="43900" windowHeight="17240" xr2:uid="{20C69EFE-B5CA-054C-B003-C53B6B330297}"/>
+    <workbookView xWindow="360" yWindow="780" windowWidth="47000" windowHeight="13900" xr2:uid="{20C69EFE-B5CA-054C-B003-C53B6B330297}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="167">
   <si>
     <t>title</t>
     <phoneticPr fontId="1"/>
@@ -644,113 +644,106 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>千種区、名古屋市、日本</t>
-    <rPh sb="0" eb="52">
+    <t>愛知県名古屋市千種区</t>
+    <rPh sb="0" eb="2">
+      <t>アイチケンナゴヤシ</t>
+    </rPh>
+    <rPh sb="64" eb="105">
       <t>チクサク</t>
     </rPh>
-    <rPh sb="106" eb="108">
+    <rPh sb="159" eb="161">
       <t>ナゴヤ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>東区、名古屋市、日本</t>
-    <rPh sb="0" eb="31">
+    <t>京都府京都市左京区</t>
+    <rPh sb="0" eb="2">
+      <t>キョウトフキョウトシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>千葉県船橋市</t>
+    <rPh sb="0" eb="2">
+      <t>チバケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>千葉県柏市</t>
+    <rPh sb="0" eb="1">
+      <t>チバケンカシワシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>京都府木津川市</t>
+    <rPh sb="0" eb="1">
+      <t>キョウトフキヅガワシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>東京都文京区</t>
+    <rPh sb="0" eb="1">
+      <t>トウキョウト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大阪府豊中市</t>
+    <rPh sb="0" eb="2">
+      <t>オオサカフ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>山梨県山中湖村</t>
+    <rPh sb="0" eb="2">
+      <t>ヤマナシケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>神奈川県箱根町</t>
+    <rPh sb="0" eb="2">
+      <t>カナガワケンハコネマチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>兵庫県篠山市</t>
+    <rPh sb="0" eb="2">
+      <t>ヒョウゴケン</t>
+    </rPh>
+    <rPh sb="21" eb="48">
+      <t>ササヤマシ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ヒョウゴ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>名古屋市東区</t>
+    <rPh sb="0" eb="2">
+      <t>ナゴヤシヒガシク</t>
+    </rPh>
+    <rPh sb="21" eb="42">
       <t>ヒガシク</t>
     </rPh>
-    <rPh sb="34" eb="35">
+    <rPh sb="45" eb="46">
       <t>ナゴヤ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>左京区、京都市、日本</t>
-    <rPh sb="0" eb="37">
-      <t>サキョウク</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>キョウト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>船橋市、千葉県、日本</t>
-    <rPh sb="0" eb="31">
-      <t>フナバシシ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>チバ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>柏市、千葉県、日本</t>
-    <rPh sb="0" eb="27">
-      <t>カシワシ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>チバ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>文京区、東京都、日本</t>
-    <rPh sb="0" eb="31">
-      <t>ブンキョウク</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>トウキョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>豊中市、大阪府、日本</t>
-    <rPh sb="0" eb="61">
-      <t>トヨナカシ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>オオサカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>山中湖村、山梨県、日本</t>
-    <rPh sb="0" eb="48">
-      <t>ヤマナカコムラ</t>
-    </rPh>
-    <rPh sb="51" eb="52">
-      <t>ヤマナシニホン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>木津川市、京都府、日本</t>
-    <rPh sb="0" eb="48">
-      <t>キヅガワシ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>キョウト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>箱根町、神奈川県、日本</t>
-    <rPh sb="0" eb="42">
-      <t>ハコネマチ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>カナガワケン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>篠山市、兵庫県、日本</t>
-    <rPh sb="0" eb="37">
-      <t>ササヤマシ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>ヒョウゴ</t>
-    </rPh>
+    <t>latitude</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>longitude</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1178,11 +1171,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899EF045-7AA2-474D-80F3-6F954183DE84}">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1191,10 +1184,10 @@
     <col min="2" max="2" width="53.28515625" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.140625" customWidth="1"/>
+    <col min="7" max="9" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1217,13 +1210,19 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="23">
+    <row r="2" spans="1:11" ht="23">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1243,11 +1242,11 @@
       <c r="G2" t="s">
         <v>154</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="23">
+    <row r="3" spans="1:11" ht="23">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1267,11 +1266,11 @@
       <c r="G3" t="s">
         <v>154</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="23">
+    <row r="4" spans="1:11" ht="23">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1289,13 +1288,13 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="23">
+    <row r="5" spans="1:11" ht="23">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1313,13 +1312,13 @@
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>156</v>
-      </c>
-      <c r="I5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="23">
+    <row r="6" spans="1:11" ht="23">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1337,13 +1336,13 @@
         <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
-      </c>
-      <c r="I6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="23">
+    <row r="7" spans="1:11" ht="23">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1361,13 +1360,13 @@
         <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>156</v>
-      </c>
-      <c r="I7" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="23">
+    <row r="8" spans="1:11" ht="23">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1385,13 +1384,13 @@
         <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>157</v>
-      </c>
-      <c r="I8" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="23">
+    <row r="9" spans="1:11" ht="23">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1411,11 +1410,11 @@
       <c r="G9" t="s">
         <v>154</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="23">
+    <row r="10" spans="1:11" ht="23">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1435,11 +1434,11 @@
       <c r="G10" t="s">
         <v>154</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="23">
+    <row r="11" spans="1:11" ht="23">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1459,11 +1458,11 @@
       <c r="G11" t="s">
         <v>154</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="23">
+    <row r="12" spans="1:11" ht="23">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
@@ -1481,13 +1480,13 @@
         <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>158</v>
-      </c>
-      <c r="I12" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="23">
+    <row r="13" spans="1:11" ht="23">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -1505,13 +1504,13 @@
         <v>79</v>
       </c>
       <c r="G13" t="s">
-        <v>156</v>
-      </c>
-      <c r="I13" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="23">
+    <row r="14" spans="1:11" ht="23">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -1529,13 +1528,13 @@
         <v>81</v>
       </c>
       <c r="G14" t="s">
-        <v>156</v>
-      </c>
-      <c r="I14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="23">
+    <row r="15" spans="1:11" ht="23">
       <c r="A15" s="5" t="s">
         <v>85</v>
       </c>
@@ -1553,13 +1552,13 @@
         <v>84</v>
       </c>
       <c r="G15" t="s">
-        <v>162</v>
-      </c>
-      <c r="I15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="23">
+    <row r="16" spans="1:11" ht="23">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -1577,13 +1576,13 @@
         <v>84</v>
       </c>
       <c r="G16" t="s">
-        <v>162</v>
-      </c>
-      <c r="I16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="23">
+    <row r="17" spans="1:11" ht="23">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -1603,11 +1602,11 @@
       <c r="G17" t="s">
         <v>159</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="23">
+    <row r="18" spans="1:11" ht="23">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -1625,13 +1624,13 @@
         <v>82</v>
       </c>
       <c r="G18" t="s">
-        <v>156</v>
-      </c>
-      <c r="I18" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="23">
+    <row r="19" spans="1:11" ht="23">
       <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
@@ -1649,13 +1648,13 @@
         <v>82</v>
       </c>
       <c r="G19" t="s">
-        <v>156</v>
-      </c>
-      <c r="I19" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="23">
+    <row r="20" spans="1:11" ht="23">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -1675,11 +1674,11 @@
       <c r="G20" t="s">
         <v>159</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="23">
+    <row r="21" spans="1:11" ht="23">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -1697,13 +1696,13 @@
         <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I21" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="23">
+    <row r="22" spans="1:11" ht="23">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -1723,11 +1722,11 @@
       <c r="G22" t="s">
         <v>160</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="23">
+    <row r="23" spans="1:11" ht="23">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -1745,13 +1744,13 @@
         <v>91</v>
       </c>
       <c r="G23" t="s">
-        <v>162</v>
-      </c>
-      <c r="I23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="23">
+    <row r="24" spans="1:11" ht="23">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -1771,11 +1770,13 @@
       <c r="G24" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="23">
+    <row r="25" spans="1:11" ht="23">
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
@@ -1795,11 +1796,11 @@
       <c r="G25" t="s">
         <v>159</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="23">
+    <row r="26" spans="1:11" ht="23">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -1819,11 +1820,11 @@
       <c r="G26" t="s">
         <v>154</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="23">
+    <row r="27" spans="1:11" ht="23">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -1843,11 +1844,11 @@
       <c r="G27" t="s">
         <v>154</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="23">
+    <row r="28" spans="1:11" ht="23">
       <c r="A28" s="7" t="s">
         <v>88</v>
       </c>
@@ -1865,13 +1866,13 @@
         <v>89</v>
       </c>
       <c r="G28" t="s">
-        <v>162</v>
-      </c>
-      <c r="I28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="23">
+    <row r="29" spans="1:11" ht="23">
       <c r="A29" s="7" t="s">
         <v>90</v>
       </c>
@@ -1889,13 +1890,13 @@
         <v>91</v>
       </c>
       <c r="G29" t="s">
-        <v>162</v>
-      </c>
-      <c r="I29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="23">
+    <row r="30" spans="1:11" ht="23">
       <c r="A30" s="1" t="s">
         <v>101</v>
       </c>
@@ -1915,11 +1916,11 @@
       <c r="G30" t="s">
         <v>154</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="23">
+    <row r="31" spans="1:11" ht="23">
       <c r="A31" s="1" t="s">
         <v>102</v>
       </c>
@@ -1939,11 +1940,11 @@
       <c r="G31" t="s">
         <v>154</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="23">
+    <row r="32" spans="1:11" ht="23">
       <c r="A32" s="1" t="s">
         <v>104</v>
       </c>
@@ -1961,13 +1962,13 @@
         <v>150</v>
       </c>
       <c r="G32" t="s">
-        <v>156</v>
-      </c>
-      <c r="I32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K32" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="23">
+    <row r="33" spans="1:11" ht="23">
       <c r="A33" s="1" t="s">
         <v>106</v>
       </c>
@@ -1985,13 +1986,13 @@
         <v>144</v>
       </c>
       <c r="G33" t="s">
-        <v>163</v>
-      </c>
-      <c r="I33" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="23">
+    <row r="34" spans="1:11" ht="23">
       <c r="A34" s="1" t="s">
         <v>109</v>
       </c>
@@ -2009,13 +2010,13 @@
         <v>143</v>
       </c>
       <c r="G34" t="s">
-        <v>156</v>
-      </c>
-      <c r="I34" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K34" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="23">
+    <row r="35" spans="1:11" ht="23">
       <c r="A35" s="1" t="s">
         <v>116</v>
       </c>
@@ -2035,11 +2036,11 @@
       <c r="G35" t="s">
         <v>154</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="23">
+    <row r="36" spans="1:11" ht="23">
       <c r="A36" s="1" t="s">
         <v>117</v>
       </c>
@@ -2059,11 +2060,11 @@
       <c r="G36" t="s">
         <v>154</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="23">
+    <row r="37" spans="1:11" ht="23">
       <c r="A37" s="1" t="s">
         <v>118</v>
       </c>
@@ -2081,13 +2082,13 @@
         <v>146</v>
       </c>
       <c r="G37" t="s">
-        <v>158</v>
-      </c>
-      <c r="I37" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="23">
+    <row r="38" spans="1:11" ht="23">
       <c r="A38" s="1" t="s">
         <v>121</v>
       </c>
@@ -2107,11 +2108,11 @@
       <c r="G38" t="s">
         <v>154</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="23">
+    <row r="39" spans="1:11" ht="23">
       <c r="A39" s="1" t="s">
         <v>122</v>
       </c>
@@ -2131,11 +2132,11 @@
       <c r="G39" t="s">
         <v>154</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="23">
+    <row r="40" spans="1:11" ht="23">
       <c r="A40" s="1" t="s">
         <v>123</v>
       </c>
@@ -2155,11 +2156,11 @@
       <c r="G40" t="s">
         <v>154</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="23">
+    <row r="41" spans="1:11" ht="23">
       <c r="A41" s="1" t="s">
         <v>124</v>
       </c>
@@ -2179,11 +2180,11 @@
       <c r="G41" t="s">
         <v>154</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="23">
+    <row r="42" spans="1:11" ht="23">
       <c r="A42" s="1" t="s">
         <v>129</v>
       </c>
@@ -2201,13 +2202,15 @@
         <v>126</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="I42" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="K42" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="23">
+    <row r="43" spans="1:11" ht="23">
       <c r="A43" s="1" t="s">
         <v>130</v>
       </c>
@@ -2225,13 +2228,13 @@
         <v>148</v>
       </c>
       <c r="G43" t="s">
-        <v>156</v>
-      </c>
-      <c r="I43" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K43" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="23">
+    <row r="44" spans="1:11" ht="23">
       <c r="A44" s="1" t="s">
         <v>133</v>
       </c>
@@ -2249,13 +2252,15 @@
         <v>141</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="I44" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="K44" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="23">
+    <row r="45" spans="1:11" ht="23">
       <c r="A45" s="1" t="s">
         <v>135</v>
       </c>
@@ -2273,13 +2278,15 @@
         <v>142</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="I45" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="K45" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="23">
+    <row r="46" spans="1:11" ht="23">
       <c r="A46" s="1" t="s">
         <v>135</v>
       </c>
@@ -2297,19 +2304,19 @@
         <v>153</v>
       </c>
       <c r="G46" t="s">
-        <v>156</v>
-      </c>
-      <c r="I46" t="s">
+        <v>155</v>
+      </c>
+      <c r="K46" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:11">
       <c r="D47" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:11">
       <c r="D48" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
add manual entries (talkmap)
</commit_message>
<xml_diff>
--- a/markdown_generator/talks.xlsx
+++ b/markdown_generator/talks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuk/git-web/stsykw.github.io/markdown_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1025E0-CBE6-364F-A45A-1A9EF4A0D193}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{8111F715-FC5E-CA4D-A4DD-D9226EFB67B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="780" windowWidth="47000" windowHeight="13900" xr2:uid="{20C69EFE-B5CA-054C-B003-C53B6B330297}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -646,13 +647,7 @@
   <si>
     <t>愛知県名古屋市千種区</t>
     <rPh sb="0" eb="2">
-      <t>アイチケンナゴヤシ</t>
-    </rPh>
-    <rPh sb="64" eb="105">
-      <t>チクサク</t>
-    </rPh>
-    <rPh sb="159" eb="161">
-      <t>ナゴヤ</t>
+      <t>アイチケンナゴヤシチクサクナゴヤ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -715,26 +710,14 @@
   <si>
     <t>兵庫県篠山市</t>
     <rPh sb="0" eb="2">
-      <t>ヒョウゴケン</t>
-    </rPh>
-    <rPh sb="21" eb="48">
-      <t>ササヤマシ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>ヒョウゴ</t>
+      <t>ヒョウゴケンササヤマシヒョウゴ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>名古屋市東区</t>
     <rPh sb="0" eb="2">
-      <t>ナゴヤシヒガシク</t>
-    </rPh>
-    <rPh sb="21" eb="42">
-      <t>ヒガシク</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ナゴヤ</t>
+      <t>ナゴヤシヒガシクヒガシクナゴヤ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -829,7 +812,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -855,6 +838,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1174,8 +1160,8 @@
   <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1242,6 +1228,12 @@
       <c r="G2" t="s">
         <v>154</v>
       </c>
+      <c r="H2">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I2">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
@@ -1266,6 +1258,12 @@
       <c r="G3" t="s">
         <v>154</v>
       </c>
+      <c r="H3">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I3">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1290,6 +1288,12 @@
       <c r="G4" t="s">
         <v>155</v>
       </c>
+      <c r="H4">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I4">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1314,6 +1318,12 @@
       <c r="G5" t="s">
         <v>155</v>
       </c>
+      <c r="H5">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I5">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1338,6 +1348,12 @@
       <c r="G6" t="s">
         <v>155</v>
       </c>
+      <c r="H6">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I6">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1362,6 +1378,12 @@
       <c r="G7" t="s">
         <v>155</v>
       </c>
+      <c r="H7">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I7">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1386,6 +1408,12 @@
       <c r="G8" t="s">
         <v>156</v>
       </c>
+      <c r="H8" s="9">
+        <v>35.726208</v>
+      </c>
+      <c r="I8">
+        <v>140.05860000000001</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1410,6 +1438,12 @@
       <c r="G9" t="s">
         <v>154</v>
       </c>
+      <c r="H9">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I9">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1434,6 +1468,12 @@
       <c r="G10" t="s">
         <v>154</v>
       </c>
+      <c r="H10">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I10">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1458,6 +1498,12 @@
       <c r="G11" t="s">
         <v>154</v>
       </c>
+      <c r="H11">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I11">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K11" s="1" t="s">
         <v>37</v>
       </c>
@@ -1482,6 +1528,12 @@
       <c r="G12" t="s">
         <v>157</v>
       </c>
+      <c r="H12">
+        <v>35.9014411</v>
+      </c>
+      <c r="I12">
+        <v>139.93639160000001</v>
+      </c>
       <c r="K12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1506,6 +1558,12 @@
       <c r="G13" t="s">
         <v>155</v>
       </c>
+      <c r="H13">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I13">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K13" s="1" t="s">
         <v>46</v>
       </c>
@@ -1530,6 +1588,12 @@
       <c r="G14" t="s">
         <v>155</v>
       </c>
+      <c r="H14">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I14">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K14" s="1" t="s">
         <v>51</v>
       </c>
@@ -1554,6 +1618,12 @@
       <c r="G15" t="s">
         <v>158</v>
       </c>
+      <c r="H15">
+        <v>34.741410299999998</v>
+      </c>
+      <c r="I15">
+        <v>135.7753898</v>
+      </c>
       <c r="K15" s="1" t="s">
         <v>94</v>
       </c>
@@ -1578,6 +1648,12 @@
       <c r="G16" t="s">
         <v>158</v>
       </c>
+      <c r="H16">
+        <v>34.741410299999998</v>
+      </c>
+      <c r="I16">
+        <v>135.7753898</v>
+      </c>
       <c r="K16" s="1" t="s">
         <v>94</v>
       </c>
@@ -1602,6 +1678,12 @@
       <c r="G17" t="s">
         <v>159</v>
       </c>
+      <c r="H17">
+        <v>35.712999799999999</v>
+      </c>
+      <c r="I17">
+        <v>139.76057280000001</v>
+      </c>
       <c r="K17" s="1" t="s">
         <v>99</v>
       </c>
@@ -1626,6 +1708,12 @@
       <c r="G18" t="s">
         <v>155</v>
       </c>
+      <c r="H18">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I18">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K18" s="1" t="s">
         <v>56</v>
       </c>
@@ -1650,6 +1738,12 @@
       <c r="G19" t="s">
         <v>155</v>
       </c>
+      <c r="H19">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I19">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K19" s="1" t="s">
         <v>56</v>
       </c>
@@ -1674,6 +1768,12 @@
       <c r="G20" t="s">
         <v>159</v>
       </c>
+      <c r="H20">
+        <v>35.712999799999999</v>
+      </c>
+      <c r="I20">
+        <v>139.76057280000001</v>
+      </c>
       <c r="K20" s="1" t="s">
         <v>100</v>
       </c>
@@ -1698,6 +1798,12 @@
       <c r="G21" t="s">
         <v>155</v>
       </c>
+      <c r="H21">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I21">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K21" s="1" t="s">
         <v>61</v>
       </c>
@@ -1722,6 +1828,12 @@
       <c r="G22" t="s">
         <v>160</v>
       </c>
+      <c r="H22">
+        <v>34.803782099999999</v>
+      </c>
+      <c r="I22">
+        <v>135.45411240000001</v>
+      </c>
       <c r="K22" s="1" t="s">
         <v>63</v>
       </c>
@@ -1746,6 +1858,12 @@
       <c r="G23" t="s">
         <v>158</v>
       </c>
+      <c r="H23">
+        <v>34.741410299999998</v>
+      </c>
+      <c r="I23">
+        <v>135.7753898</v>
+      </c>
       <c r="K23" s="1" t="s">
         <v>96</v>
       </c>
@@ -1770,8 +1888,12 @@
       <c r="G24" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="H24" s="3">
+        <v>35.416749000000003</v>
+      </c>
+      <c r="I24" s="3">
+        <v>138.8964995</v>
+      </c>
       <c r="K24" s="1" t="s">
         <v>95</v>
       </c>
@@ -1796,6 +1918,12 @@
       <c r="G25" t="s">
         <v>159</v>
       </c>
+      <c r="H25">
+        <v>35.712999799999999</v>
+      </c>
+      <c r="I25">
+        <v>139.76057280000001</v>
+      </c>
       <c r="K25" s="1" t="s">
         <v>67</v>
       </c>
@@ -1820,6 +1948,12 @@
       <c r="G26" t="s">
         <v>154</v>
       </c>
+      <c r="H26">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I26">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K26" s="1" t="s">
         <v>70</v>
       </c>
@@ -1844,6 +1978,12 @@
       <c r="G27" t="s">
         <v>154</v>
       </c>
+      <c r="H27">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I27">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K27" s="1" t="s">
         <v>70</v>
       </c>
@@ -1868,6 +2008,12 @@
       <c r="G28" t="s">
         <v>158</v>
       </c>
+      <c r="H28">
+        <v>34.741410299999998</v>
+      </c>
+      <c r="I28">
+        <v>135.7753898</v>
+      </c>
       <c r="K28" s="1" t="s">
         <v>94</v>
       </c>
@@ -1892,6 +2038,12 @@
       <c r="G29" t="s">
         <v>158</v>
       </c>
+      <c r="H29">
+        <v>34.741410299999998</v>
+      </c>
+      <c r="I29">
+        <v>135.7753898</v>
+      </c>
       <c r="K29" s="1" t="s">
         <v>94</v>
       </c>
@@ -1916,6 +2068,12 @@
       <c r="G30" t="s">
         <v>154</v>
       </c>
+      <c r="H30">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I30">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K30" s="1" t="s">
         <v>103</v>
       </c>
@@ -1940,6 +2098,12 @@
       <c r="G31" t="s">
         <v>154</v>
       </c>
+      <c r="H31">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I31">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K31" s="1" t="s">
         <v>103</v>
       </c>
@@ -1964,6 +2128,12 @@
       <c r="G32" t="s">
         <v>155</v>
       </c>
+      <c r="H32">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I32">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K32" s="1" t="s">
         <v>151</v>
       </c>
@@ -1988,6 +2158,12 @@
       <c r="G33" t="s">
         <v>162</v>
       </c>
+      <c r="H33">
+        <v>35.252982899999999</v>
+      </c>
+      <c r="I33">
+        <v>139.04386030000001</v>
+      </c>
       <c r="K33" s="1" t="s">
         <v>145</v>
       </c>
@@ -2012,6 +2188,12 @@
       <c r="G34" t="s">
         <v>155</v>
       </c>
+      <c r="H34">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I34">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K34" s="1" t="s">
         <v>108</v>
       </c>
@@ -2036,6 +2218,12 @@
       <c r="G35" t="s">
         <v>154</v>
       </c>
+      <c r="H35">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I35">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K35" s="1" t="s">
         <v>111</v>
       </c>
@@ -2060,6 +2248,12 @@
       <c r="G36" t="s">
         <v>154</v>
       </c>
+      <c r="H36">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I36">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K36" s="1" t="s">
         <v>112</v>
       </c>
@@ -2084,6 +2278,12 @@
       <c r="G37" t="s">
         <v>157</v>
       </c>
+      <c r="H37">
+        <v>35.9014411</v>
+      </c>
+      <c r="I37">
+        <v>139.93639160000001</v>
+      </c>
       <c r="K37" s="1" t="s">
         <v>147</v>
       </c>
@@ -2108,6 +2308,12 @@
       <c r="G38" t="s">
         <v>154</v>
       </c>
+      <c r="H38">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I38">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K38" s="1" t="s">
         <v>119</v>
       </c>
@@ -2132,6 +2338,12 @@
       <c r="G39" t="s">
         <v>154</v>
       </c>
+      <c r="H39">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I39">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K39" s="1" t="s">
         <v>119</v>
       </c>
@@ -2156,6 +2368,12 @@
       <c r="G40" t="s">
         <v>154</v>
       </c>
+      <c r="H40">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I40">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K40" s="1" t="s">
         <v>119</v>
       </c>
@@ -2180,6 +2398,12 @@
       <c r="G41" t="s">
         <v>154</v>
       </c>
+      <c r="H41">
+        <v>35.153491000000002</v>
+      </c>
+      <c r="I41">
+        <v>136.96757299999999</v>
+      </c>
       <c r="K41" s="1" t="s">
         <v>125</v>
       </c>
@@ -2204,8 +2428,12 @@
       <c r="G42" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
+      <c r="H42" s="8">
+        <v>35.032056099999998</v>
+      </c>
+      <c r="I42" s="8">
+        <v>135.3228091</v>
+      </c>
       <c r="K42" s="1" t="s">
         <v>127</v>
       </c>
@@ -2230,6 +2458,12 @@
       <c r="G43" t="s">
         <v>155</v>
       </c>
+      <c r="H43">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I43">
+        <v>135.78553289999999</v>
+      </c>
       <c r="K43" s="1" t="s">
         <v>149</v>
       </c>
@@ -2254,8 +2488,12 @@
       <c r="G44" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="H44" s="8">
+        <v>35.173737099999997</v>
+      </c>
+      <c r="I44" s="8">
+        <v>136.90776220000001</v>
+      </c>
       <c r="K44" s="1" t="s">
         <v>132</v>
       </c>
@@ -2280,8 +2518,12 @@
       <c r="G45" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
+      <c r="H45" s="8">
+        <v>35.173737099999997</v>
+      </c>
+      <c r="I45" s="8">
+        <v>136.90776220000001</v>
+      </c>
       <c r="K45" s="1" t="s">
         <v>136</v>
       </c>
@@ -2305,6 +2547,12 @@
       </c>
       <c r="G46" t="s">
         <v>155</v>
+      </c>
+      <c r="H46">
+        <v>35.030811499999999</v>
+      </c>
+      <c r="I46">
+        <v>135.78553289999999</v>
       </c>
       <c r="K46" t="s">
         <v>152</v>

</xml_diff>